<commit_message>
Update results after aggregate Orlen's target changed
</commit_message>
<xml_diff>
--- a/data/clean/output_data.xlsx
+++ b/data/clean/output_data.xlsx
@@ -10408,7 +10408,7 @@
       </c>
       <c r="I68" t="inlineStr"/>
       <c r="J68" t="n">
-        <v>0.265</v>
+        <v>0.26</v>
       </c>
       <c r="K68" t="n">
         <v>2020</v>
@@ -10504,7 +10504,7 @@
         </is>
       </c>
       <c r="AL68" t="n">
-        <v>0.0265</v>
+        <v>0.026</v>
       </c>
       <c r="AM68" t="inlineStr">
         <is>
@@ -10532,13 +10532,13 @@
         <v>0.829523459164192</v>
       </c>
       <c r="AT68" t="n">
-        <v>1.87</v>
+        <v>1.89</v>
       </c>
       <c r="AU68" t="n">
         <v>0</v>
       </c>
       <c r="AV68" t="n">
-        <v>1.87</v>
+        <v>1.89</v>
       </c>
     </row>
     <row r="69">

</xml_diff>